<commit_message>
Update ao modelo de domínio e Use Case de Escolha de Componente Primário
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponentePrimario.xlsx
+++ b/diagramas/UseCases/EscolherComponentePrimario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{94606C45-1DA9-43B4-9862-5C52F267166B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC283E1-F658-4F04-A3E6-44CE5206885B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -25,15 +25,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>Actor input</t>
   </si>
   <si>
     <t>System response</t>
-  </si>
-  <si>
-    <t>Cenário ...</t>
   </si>
   <si>
     <t>Cenário 
@@ -52,16 +49,52 @@
     <t>Pós condição:</t>
   </si>
   <si>
-    <t>1.</t>
-  </si>
-  <si>
-    <t>2.</t>
-  </si>
-  <si>
     <t>Escolher componente primário</t>
   </si>
   <si>
     <t>Utilizador</t>
+  </si>
+  <si>
+    <t>Componente primário selecionado</t>
+  </si>
+  <si>
+    <t>1. Apresenta os componentes primários disponíveis</t>
+  </si>
+  <si>
+    <t>2. Seleciona o componente específico</t>
+  </si>
+  <si>
+    <t>4. Seleciona o modelo do componente</t>
+  </si>
+  <si>
+    <t>3. Apresenta os modelos do componente</t>
+  </si>
+  <si>
+    <t>5. Apresenta o preço do modelo</t>
+  </si>
+  <si>
+    <t>6. Confirma a inclusão do componente na configuração</t>
+  </si>
+  <si>
+    <t>5.1 Apresenta os componentes extra que devem ser incluídos</t>
+  </si>
+  <si>
+    <t>5.2 Confirma a inclusão dos componentes extra</t>
+  </si>
+  <si>
+    <t>7. Adiciona o componente aos componentes selecionados</t>
+  </si>
+  <si>
+    <t>5.3 Regressa a 5</t>
+  </si>
+  <si>
+    <t>Comp. Alternativo 1 [requer componentes extra] (passo 4)</t>
+  </si>
+  <si>
+    <t>Exceção 2 [rejeita componentes extra] (passo 5.2)</t>
+  </si>
+  <si>
+    <t>5.2.1 Indica que não é possível adicionar o componente selecionado</t>
   </si>
 </sst>
 </file>
@@ -98,7 +131,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="13">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -110,6 +143,46 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -125,15 +198,86 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right/>
       <top style="medium">
         <color indexed="64"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -144,7 +288,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -153,7 +299,9 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
@@ -164,38 +312,10 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right style="medium">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top/>
       <bottom/>
       <diagonal/>
@@ -204,9 +324,7 @@
       <left style="medium">
         <color indexed="64"/>
       </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
+      <right/>
       <top/>
       <bottom style="medium">
         <color indexed="64"/>
@@ -214,87 +332,87 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right/>
-      <top style="medium">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
       <right style="medium">
         <color indexed="64"/>
       </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
+      <top/>
+      <bottom/>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -610,144 +728,213 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D19"/>
+  <dimension ref="B1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4:D4"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="16.5" customWidth="1"/>
     <col min="2" max="2" width="16.125" customWidth="1"/>
-    <col min="3" max="3" width="33.375" customWidth="1"/>
-    <col min="4" max="4" width="37.5" customWidth="1"/>
+    <col min="3" max="3" width="55.25" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="52" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D2" s="10"/>
+    </row>
+    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C2" s="11" t="s">
+      <c r="C3" s="9" t="s">
+        <v>8</v>
+      </c>
+      <c r="D3" s="10"/>
+    </row>
+    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B4" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="10"/>
+    </row>
+    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B5" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C5" s="11" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" s="12"/>
+    </row>
+    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B6" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="7" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="14"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="12"/>
-    </row>
-    <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B3" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="C3" s="11" t="s">
+    </row>
+    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B8" s="14"/>
+      <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D3" s="12"/>
-    </row>
-    <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B4" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="C4" s="11"/>
-      <c r="D4" s="12"/>
-    </row>
-    <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B5" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="14"/>
-    </row>
-    <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" s="8" t="s">
-        <v>0</v>
-      </c>
-      <c r="D6" s="9" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="16"/>
-      <c r="C7" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="16"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="1" t="s">
-        <v>9</v>
-      </c>
+      <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="16"/>
-      <c r="C9" s="5"/>
-      <c r="D9" s="1"/>
+      <c r="B9" s="14"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="16"/>
-      <c r="C10" s="5"/>
+      <c r="B10" s="14"/>
+      <c r="C10" s="4" t="s">
+        <v>12</v>
+      </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="16"/>
-      <c r="C11" s="5"/>
-      <c r="D11" s="1"/>
+      <c r="B11" s="14"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="16"/>
-      <c r="C12" s="5"/>
+      <c r="B12" s="14"/>
+      <c r="C12" s="4" t="s">
+        <v>15</v>
+      </c>
       <c r="D12" s="1"/>
     </row>
-    <row r="13" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="16"/>
-      <c r="C13" s="5"/>
-      <c r="D13" s="1"/>
+    <row r="13" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B13" s="14"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="26" t="s">
+        <v>18</v>
+      </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="16"/>
-      <c r="C14" s="5"/>
+      <c r="B14" s="14"/>
+      <c r="C14" s="4"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="16"/>
-      <c r="C15" s="5"/>
+      <c r="B15" s="14"/>
+      <c r="C15" s="4"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="16"/>
-      <c r="C16" s="6"/>
-      <c r="D16" s="3"/>
-    </row>
-    <row r="17" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="C17" s="4"/>
-      <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B18" s="10"/>
-      <c r="C18" s="5"/>
+      <c r="B16" s="15"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="2"/>
+    </row>
+    <row r="17" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
+      <c r="B17" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="C17" s="3"/>
+      <c r="D17" s="25" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B18" s="17"/>
+      <c r="C18" s="4" t="s">
+        <v>17</v>
+      </c>
       <c r="D18" s="1"/>
     </row>
-    <row r="19" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="10"/>
-      <c r="C19" s="6"/>
-      <c r="D19" s="3"/>
+    <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B19" s="23"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="24" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="17"/>
+      <c r="C20" s="21"/>
+      <c r="D20" s="19"/>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="17"/>
+      <c r="C21" s="21"/>
+      <c r="D21" s="19"/>
+    </row>
+    <row r="22" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B22" s="18"/>
+      <c r="C22" s="22"/>
+      <c r="D22" s="20"/>
+    </row>
+    <row r="23" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B23" s="27" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23" s="29"/>
+      <c r="D23" s="30" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B24" s="23"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="19"/>
+    </row>
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B25" s="23"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="19"/>
+    </row>
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B26" s="23"/>
+      <c r="C26" s="21"/>
+      <c r="D26" s="19"/>
+    </row>
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B27" s="23"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="19"/>
+    </row>
+    <row r="28" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B28" s="28"/>
+      <c r="C28" s="22"/>
+      <c r="D28" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="6">
-    <mergeCell ref="B17:B19"/>
+  <mergeCells count="7">
+    <mergeCell ref="B23:B28"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:B16"/>
+    <mergeCell ref="B17:B22"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Primeira versão dos use cases done
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponentePrimario.xlsx
+++ b/diagramas/UseCases/EscolherComponentePrimario.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAC283E1-F658-4F04-A3E6-44CE5206885B}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DD4CA4-FD6A-4AB0-9907-333D5A8FAF84}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -94,7 +94,7 @@
     <t>Exceção 2 [rejeita componentes extra] (passo 5.2)</t>
   </si>
   <si>
-    <t>5.2.1 Indica que não é possível adicionar o componente selecionado</t>
+    <t>5.2.1 Indica que não é possível adicionar o componente primário selecionado</t>
   </si>
 </sst>
 </file>
@@ -360,43 +360,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -404,15 +371,48 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -731,7 +731,7 @@
   <dimension ref="B1:D28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -747,38 +747,38 @@
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="9" t="s">
+      <c r="C2" s="21" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="10"/>
+      <c r="D2" s="22"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="10"/>
+      <c r="D3" s="22"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="10"/>
+      <c r="C4" s="21"/>
+      <c r="D4" s="22"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="12"/>
+      <c r="D5" s="24"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="13" t="s">
+      <c r="B6" s="25" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -789,140 +789,140 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="14"/>
+      <c r="B7" s="26"/>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="14"/>
+      <c r="B8" s="26"/>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="14"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="14"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="14"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="14"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="14"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="26" t="s">
+      <c r="D13" s="15" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="14"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="14"/>
+      <c r="B15" s="26"/>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="15"/>
+      <c r="B16" s="27"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="16" t="s">
+      <c r="B17" s="28" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="25" t="s">
+      <c r="D17" s="14" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="17"/>
+      <c r="B18" s="29"/>
       <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="23"/>
+      <c r="B19" s="19"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="13" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="17"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="19"/>
+      <c r="B20" s="29"/>
+      <c r="C20" s="11"/>
+      <c r="D20" s="9"/>
     </row>
     <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="17"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="19"/>
+      <c r="B21" s="29"/>
+      <c r="C21" s="11"/>
+      <c r="D21" s="9"/>
     </row>
     <row r="22" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="18"/>
-      <c r="C22" s="22"/>
-      <c r="D22" s="20"/>
+      <c r="B22" s="30"/>
+      <c r="C22" s="12"/>
+      <c r="D22" s="10"/>
     </row>
     <row r="23" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="27" t="s">
+      <c r="B23" s="18" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="29"/>
-      <c r="D23" s="30" t="s">
+      <c r="C23" s="16"/>
+      <c r="D23" s="17" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="23"/>
-      <c r="C24" s="21"/>
-      <c r="D24" s="19"/>
+      <c r="B24" s="19"/>
+      <c r="C24" s="11"/>
+      <c r="D24" s="9"/>
     </row>
     <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="23"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="19"/>
+      <c r="B25" s="19"/>
+      <c r="C25" s="11"/>
+      <c r="D25" s="9"/>
     </row>
     <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="23"/>
-      <c r="C26" s="21"/>
-      <c r="D26" s="19"/>
+      <c r="B26" s="19"/>
+      <c r="C26" s="11"/>
+      <c r="D26" s="9"/>
     </row>
     <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="23"/>
-      <c r="C27" s="21"/>
-      <c r="D27" s="19"/>
+      <c r="B27" s="19"/>
+      <c r="C27" s="11"/>
+      <c r="D27" s="9"/>
     </row>
     <row r="28" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="28"/>
-      <c r="C28" s="22"/>
-      <c r="D28" s="20"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="12"/>
+      <c r="D28" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="7">

</xml_diff>

<commit_message>
Atualizei alguns use cases e fiz um diagrama de máquina de estado
Para além disso, também esquematizei o nosso mapa de navegação no ConfiguraFacil
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponentePrimario.xlsx
+++ b/diagramas/UseCases/EscolherComponentePrimario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6DD4CA4-FD6A-4AB0-9907-333D5A8FAF84}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6585C49-9CE1-49F2-AAFB-B053C8EFA330}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -346,7 +346,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -360,9 +360,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -375,15 +373,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -405,13 +394,22 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -728,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D28"/>
+  <dimension ref="B1:D22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -747,38 +745,38 @@
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="21" t="s">
+      <c r="C2" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="22"/>
+      <c r="D2" s="17"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="21" t="s">
+      <c r="C3" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="22"/>
+      <c r="D3" s="17"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="22"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="17"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="24"/>
+      <c r="D5" s="19"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="20" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -789,150 +787,120 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="26"/>
+      <c r="B7" s="21"/>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="26"/>
+      <c r="B8" s="21"/>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="26"/>
+      <c r="B9" s="21"/>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="26"/>
+      <c r="B10" s="21"/>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="26"/>
+      <c r="B11" s="21"/>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="26"/>
+      <c r="B12" s="21"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="26"/>
+      <c r="B13" s="21"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="15" t="s">
+      <c r="D13" s="13" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="26"/>
+      <c r="B14" s="21"/>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="26"/>
+      <c r="B15" s="21"/>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="27"/>
+      <c r="B16" s="22"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="28" t="s">
+      <c r="B17" s="25" t="s">
         <v>20</v>
       </c>
       <c r="C17" s="3"/>
-      <c r="D17" s="14" t="s">
+      <c r="D17" s="12" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="29"/>
+      <c r="B18" s="26"/>
       <c r="C18" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="19"/>
+      <c r="B19" s="27"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="13" t="s">
+      <c r="D19" s="11" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B20" s="29"/>
-      <c r="C20" s="11"/>
+    <row r="20" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="28"/>
+      <c r="C20" s="10"/>
       <c r="D20" s="9"/>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B21" s="29"/>
-      <c r="C21" s="11"/>
-      <c r="D21" s="9"/>
+    <row r="21" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B21" s="23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C21" s="14"/>
+      <c r="D21" s="15" t="s">
+        <v>22</v>
+      </c>
     </row>
     <row r="22" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="30"/>
-      <c r="C22" s="12"/>
-      <c r="D22" s="10"/>
-    </row>
-    <row r="23" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B23" s="18" t="s">
-        <v>21</v>
-      </c>
-      <c r="C23" s="16"/>
-      <c r="D23" s="17" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B24" s="19"/>
-      <c r="C24" s="11"/>
-      <c r="D24" s="9"/>
-    </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B25" s="19"/>
-      <c r="C25" s="11"/>
-      <c r="D25" s="9"/>
-    </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B26" s="19"/>
-      <c r="C26" s="11"/>
-      <c r="D26" s="9"/>
-    </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B27" s="19"/>
-      <c r="C27" s="11"/>
-      <c r="D27" s="9"/>
-    </row>
-    <row r="28" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B28" s="20"/>
-      <c r="C28" s="12"/>
-      <c r="D28" s="10"/>
+      <c r="B22" s="24"/>
+      <c r="C22" s="10"/>
+      <c r="D22" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="7">
-    <mergeCell ref="B23:B28"/>
+    <mergeCell ref="B21:B22"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
     <mergeCell ref="C4:D4"/>
     <mergeCell ref="C5:D5"/>
     <mergeCell ref="B6:B16"/>
-    <mergeCell ref="B17:B22"/>
+    <mergeCell ref="B17:B20"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Escolher Componente Primário atualizado para prever incompatibilidades
Atualização de Use Case, Diagrama de Máquina de Estado e Mockup
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponentePrimario.xlsx
+++ b/diagramas/UseCases/EscolherComponentePrimario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F6585C49-9CE1-49F2-AAFB-B053C8EFA330}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36360E36-7B96-47BC-B6B3-00178731F030}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="27">
   <si>
     <t>Actor input</t>
   </si>
@@ -76,34 +76,53 @@
     <t>6. Confirma a inclusão do componente na configuração</t>
   </si>
   <si>
-    <t>5.1 Apresenta os componentes extra que devem ser incluídos</t>
-  </si>
-  <si>
-    <t>5.2 Confirma a inclusão dos componentes extra</t>
-  </si>
-  <si>
     <t>7. Adiciona o componente aos componentes selecionados</t>
   </si>
   <si>
-    <t>5.3 Regressa a 5</t>
-  </si>
-  <si>
     <t>Comp. Alternativo 1 [requer componentes extra] (passo 4)</t>
   </si>
   <si>
-    <t>Exceção 2 [rejeita componentes extra] (passo 5.2)</t>
-  </si>
-  <si>
     <t>5.2.1 Indica que não é possível adicionar o componente primário selecionado</t>
+  </si>
+  <si>
+    <t>Comp. Alternativo 3 [novo componente incompatível com componentes já selecionados] (passo 5)</t>
+  </si>
+  <si>
+    <t>4.1 Apresenta os componentes extra que devem ser incluídos</t>
+  </si>
+  <si>
+    <t>4.2 Confirma a inclusão dos componentes extra</t>
+  </si>
+  <si>
+    <t>5.2 Confirma a remoção desses componentes</t>
+  </si>
+  <si>
+    <t>5.3 Volta a 5</t>
+  </si>
+  <si>
+    <t>Exceção 2 [rejeita componentes extra] (passo 4.2)</t>
+  </si>
+  <si>
+    <t>Exceção 4 [rejeita componentes extra] (passo 5.2)</t>
+  </si>
+  <si>
+    <t>5.1 Apresenta componentes que são incompatíveis</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -131,7 +150,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -342,48 +361,90 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -394,23 +455,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -726,10 +772,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1247600E-1397-C742-A058-B663B513FA0A}">
-  <dimension ref="B1:D22"/>
+  <dimension ref="B1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -776,7 +822,7 @@
       <c r="D5" s="19"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B6" s="20" t="s">
+      <c r="B6" s="28" t="s">
         <v>2</v>
       </c>
       <c r="C6" s="7" t="s">
@@ -787,113 +833,160 @@
       </c>
     </row>
     <row r="7" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="21"/>
+      <c r="B7" s="29"/>
       <c r="C7" s="4"/>
       <c r="D7" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="21"/>
+      <c r="B8" s="29"/>
       <c r="C8" s="4" t="s">
         <v>11</v>
       </c>
       <c r="D8" s="1"/>
     </row>
     <row r="9" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="21"/>
+      <c r="B9" s="29"/>
       <c r="C9" s="4"/>
       <c r="D9" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B10" s="21"/>
+      <c r="B10" s="29"/>
       <c r="C10" s="4" t="s">
         <v>12</v>
       </c>
       <c r="D10" s="1"/>
     </row>
     <row r="11" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B11" s="21"/>
+      <c r="B11" s="29"/>
       <c r="C11" s="4"/>
       <c r="D11" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="12" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B12" s="21"/>
+      <c r="B12" s="29"/>
       <c r="C12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="D12" s="1"/>
     </row>
     <row r="13" spans="2:4" ht="38.25" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B13" s="21"/>
+      <c r="B13" s="29"/>
       <c r="C13" s="4"/>
       <c r="D13" s="13" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B14" s="21"/>
+      <c r="B14" s="29"/>
       <c r="C14" s="4"/>
       <c r="D14" s="1"/>
     </row>
     <row r="15" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B15" s="21"/>
+      <c r="B15" s="29"/>
       <c r="C15" s="4"/>
       <c r="D15" s="1"/>
     </row>
     <row r="16" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B16" s="22"/>
+      <c r="B16" s="30"/>
       <c r="C16" s="5"/>
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="25" t="s">
-        <v>20</v>
+      <c r="B17" s="22" t="s">
+        <v>17</v>
       </c>
       <c r="C17" s="3"/>
       <c r="D17" s="12" t="s">
-        <v>16</v>
+        <v>20</v>
       </c>
     </row>
     <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="26"/>
+      <c r="B18" s="23"/>
       <c r="C18" s="4" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B19" s="27"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="11" t="s">
-        <v>19</v>
-      </c>
+      <c r="D19" s="31"/>
     </row>
     <row r="20" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="28"/>
+      <c r="B20" s="24"/>
       <c r="C20" s="10"/>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="23" t="s">
-        <v>21</v>
+      <c r="B21" s="25" t="s">
+        <v>24</v>
       </c>
       <c r="C21" s="14"/>
       <c r="D21" s="15" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="24"/>
+      <c r="B22" s="26"/>
       <c r="C22" s="10"/>
       <c r="D22" s="9"/>
     </row>
+    <row r="23" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B23" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="C23" s="20"/>
+      <c r="D23" s="12" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B24" s="23"/>
+      <c r="C24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D24" s="1"/>
+    </row>
+    <row r="25" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B25" s="23"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="26" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B26" s="23"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="11"/>
+    </row>
+    <row r="27" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B27" s="24"/>
+      <c r="C27" s="21"/>
+      <c r="D27" s="9"/>
+    </row>
+    <row r="28" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B28" s="25" t="s">
+        <v>25</v>
+      </c>
+      <c r="C28" s="14"/>
+      <c r="D28" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="26"/>
+      <c r="C29" s="10"/>
+      <c r="D29" s="9"/>
+    </row>
   </sheetData>
-  <mergeCells count="7">
+  <mergeCells count="9">
+    <mergeCell ref="B23:B27"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="B21:B22"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>

</xml_diff>

<commit_message>
Atualização ao User Case Componente Primário
</commit_message>
<xml_diff>
--- a/diagramas/UseCases/EscolherComponentePrimario.xlsx
+++ b/diagramas/UseCases/EscolherComponentePrimario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Documents\GitHub\Configura-Facil\diagramas\UseCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36360E36-7B96-47BC-B6B3-00178731F030}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{354708CE-AB71-410E-8A45-B282AEEFE8AC}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{C7A0A64F-69DF-CB43-BB66-CA0002FD1B4D}"/>
   </bookViews>
@@ -103,19 +103,26 @@
     <t>Exceção 2 [rejeita componentes extra] (passo 4.2)</t>
   </si>
   <si>
-    <t>Exceção 4 [rejeita componentes extra] (passo 5.2)</t>
-  </si>
-  <si>
     <t>5.1 Apresenta componentes que são incompatíveis</t>
+  </si>
+  <si>
+    <t>Exceção 4 [rejeita remoção de incompatibilidades] (passo 5.2)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -387,76 +394,79 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -775,7 +785,7 @@
   <dimension ref="B1:D29"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -791,35 +801,35 @@
       <c r="B2" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="24" t="s">
         <v>7</v>
       </c>
-      <c r="D2" s="17"/>
+      <c r="D2" s="25"/>
     </row>
     <row r="3" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="16" t="s">
+      <c r="C3" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="D3" s="17"/>
+      <c r="D3" s="25"/>
     </row>
     <row r="4" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B4" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C4" s="16"/>
-      <c r="D4" s="17"/>
+      <c r="C4" s="24"/>
+      <c r="D4" s="25"/>
     </row>
     <row r="5" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C5" s="18" t="s">
+      <c r="C5" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="D5" s="19"/>
+      <c r="D5" s="27"/>
     </row>
     <row r="6" spans="2:4" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B6" s="28" t="s">
@@ -897,7 +907,7 @@
       <c r="D16" s="2"/>
     </row>
     <row r="17" spans="2:4" ht="37.5" x14ac:dyDescent="0.3">
-      <c r="B17" s="22" t="s">
+      <c r="B17" s="19" t="s">
         <v>17</v>
       </c>
       <c r="C17" s="3"/>
@@ -906,24 +916,24 @@
       </c>
     </row>
     <row r="18" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B18" s="23"/>
+      <c r="B18" s="20"/>
       <c r="C18" s="4" t="s">
         <v>21</v>
       </c>
       <c r="D18" s="1"/>
     </row>
     <row r="19" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B19" s="27"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="4"/>
-      <c r="D19" s="31"/>
+      <c r="D19" s="18"/>
     </row>
     <row r="20" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="24"/>
+      <c r="B20" s="21"/>
       <c r="C20" s="10"/>
       <c r="D20" s="9"/>
     </row>
     <row r="21" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B21" s="25" t="s">
+      <c r="B21" s="22" t="s">
         <v>24</v>
       </c>
       <c r="C21" s="14"/>
@@ -932,54 +942,54 @@
       </c>
     </row>
     <row r="22" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B22" s="26"/>
+      <c r="B22" s="23"/>
       <c r="C22" s="10"/>
       <c r="D22" s="9"/>
     </row>
     <row r="23" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B23" s="22" t="s">
+      <c r="B23" s="19" t="s">
         <v>19</v>
       </c>
-      <c r="C23" s="20"/>
+      <c r="C23" s="16"/>
       <c r="D23" s="12" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B24" s="23"/>
+      <c r="B24" s="20"/>
       <c r="C24" s="4" t="s">
         <v>22</v>
       </c>
       <c r="D24" s="1"/>
     </row>
     <row r="25" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B25" s="23"/>
+      <c r="B25" s="20"/>
       <c r="C25" s="4"/>
       <c r="D25" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="26" spans="2:4" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="B26" s="23"/>
+      <c r="B26" s="20"/>
       <c r="C26" s="4"/>
       <c r="D26" s="11"/>
     </row>
     <row r="27" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B27" s="24"/>
-      <c r="C27" s="21"/>
+      <c r="B27" s="21"/>
+      <c r="C27" s="17"/>
       <c r="D27" s="9"/>
     </row>
     <row r="28" spans="2:4" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="B28" s="25" t="s">
-        <v>25</v>
+      <c r="B28" s="32" t="s">
+        <v>26</v>
       </c>
       <c r="C28" s="14"/>
       <c r="D28" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="29" spans="2:4" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B29" s="26"/>
+    <row r="29" spans="2:4" ht="30.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="23"/>
       <c r="C29" s="10"/>
       <c r="D29" s="9"/>
     </row>

</xml_diff>